<commit_message>
GIMBAL: fix PCBWay BOM
</commit_message>
<xml_diff>
--- a/Projects/Gimbal/Rev2/Gimbal BOM PCBWay.xlsx
+++ b/Projects/Gimbal/Rev2/Gimbal BOM PCBWay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lance\Github\MarsRover2020-PCB\Projects\Gimbal\Rev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{310428D8-1856-469F-91AE-CB2AEA4E191B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C964E40-5761-4595-87AC-64ECD9B82F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="18000" windowHeight="9398" xr2:uid="{5AAE0AEF-46A0-4516-82AC-C6EA8D82BD9A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{5AAE0AEF-46A0-4516-82AC-C6EA8D82BD9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Gimbal BOM PCBWay" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="164">
   <si>
     <t>Line #</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>SOT-563</t>
+  </si>
+  <si>
+    <t>64-LQFP</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,9 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -971,8 +976,12 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">

</xml_diff>